<commit_message>
can auto generate excel sheets for any given official competition.
</commit_message>
<xml_diff>
--- a/ScoutingComplex2015/DataEntry/template.xlsx
+++ b/ScoutingComplex2015/DataEntry/template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aravindkoneru/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aravindkoneru/Desktop/Scouting System/ScoutingComplex2015/DataEntry/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,27 +24,72 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
-  <si>
-    <t>totes stacked</t>
-  </si>
-  <si>
-    <t>bins stacked</t>
-  </si>
-  <si>
-    <t>coopertition points</t>
-  </si>
-  <si>
-    <t>bins w/ noodle stacked</t>
-  </si>
-  <si>
-    <t>landfill</t>
-  </si>
-  <si>
-    <t>litter thrown</t>
-  </si>
-  <si>
-    <t>feeder</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="22">
+  <si>
+    <t>interaction</t>
+  </si>
+  <si>
+    <t>totes</t>
+  </si>
+  <si>
+    <t>bins</t>
+  </si>
+  <si>
+    <t>actionsAttempted</t>
+  </si>
+  <si>
+    <t>robotSet</t>
+  </si>
+  <si>
+    <t>containerSet</t>
+  </si>
+  <si>
+    <t>toteSet</t>
+  </si>
+  <si>
+    <t>stackedToteSet</t>
+  </si>
+  <si>
+    <t>actionsCompleted</t>
+  </si>
+  <si>
+    <t>teleOp</t>
+  </si>
+  <si>
+    <t>totesStacked</t>
+  </si>
+  <si>
+    <t>totesHP</t>
+  </si>
+  <si>
+    <t>totesLandfill</t>
+  </si>
+  <si>
+    <t>size1</t>
+  </si>
+  <si>
+    <t>size2</t>
+  </si>
+  <si>
+    <t>size3</t>
+  </si>
+  <si>
+    <t>size4</t>
+  </si>
+  <si>
+    <t>size5</t>
+  </si>
+  <si>
+    <t>size6</t>
+  </si>
+  <si>
+    <t>coop</t>
+  </si>
+  <si>
+    <t>obtained</t>
+  </si>
+  <si>
+    <t>step</t>
   </si>
 </sst>
 </file>
@@ -93,17 +138,29 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="9">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -379,9 +436,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:U2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -390,29 +449,97 @@
     <col min="3" max="3" width="19.83203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
       <c r="C1" t="s">
         <v>3</v>
       </c>
-      <c r="D1" t="s">
+      <c r="G1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" t="s">
+        <v>9</v>
+      </c>
+      <c r="N1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
+      <c r="T1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" t="s">
         <v>5</v>
       </c>
-      <c r="F1" t="s">
+      <c r="E2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G2" t="s">
         <v>4</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H2" t="s">
+        <v>5</v>
+      </c>
+      <c r="I2" t="s">
         <v>6</v>
+      </c>
+      <c r="J2" t="s">
+        <v>7</v>
+      </c>
+      <c r="K2" t="s">
+        <v>10</v>
+      </c>
+      <c r="L2" t="s">
+        <v>11</v>
+      </c>
+      <c r="M2" t="s">
+        <v>12</v>
+      </c>
+      <c r="N2" t="s">
+        <v>13</v>
+      </c>
+      <c r="O2" t="s">
+        <v>14</v>
+      </c>
+      <c r="P2" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>16</v>
+      </c>
+      <c r="R2" t="s">
+        <v>17</v>
+      </c>
+      <c r="S2" t="s">
+        <v>18</v>
+      </c>
+      <c r="T2" t="s">
+        <v>20</v>
+      </c>
+      <c r="U2" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>